<commit_message>
Remove internal columns from database.
</commit_message>
<xml_diff>
--- a/data/database-column-definitions.xlsx
+++ b/data/database-column-definitions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>phylum</t>
   </si>
@@ -132,18 +132,6 @@
     <t>original brain size - units</t>
   </si>
   <si>
-    <t>observationID</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>modified</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -259,18 +247,6 @@
   </si>
   <si>
     <t>Unstandardised brain size from source document</t>
-  </si>
-  <si>
-    <t>Used internally to track observations back to source data: raw file name</t>
-  </si>
-  <si>
-    <t>Used internally to track observations back to source data: raw file line number</t>
-  </si>
-  <si>
-    <t>Used internally to track observations back to source data: observation ID</t>
-  </si>
-  <si>
-    <t>Used internally to track observations back to source data: raw file modification time at time of database compilation</t>
   </si>
 </sst>
 </file>
@@ -610,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,13 +601,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,10 +626,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,10 +637,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -703,10 +679,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,10 +690,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,7 +712,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +728,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +736,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +744,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -776,7 +752,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +760,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +768,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +776,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,7 +800,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,7 +808,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +816,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +824,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -856,7 +832,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +840,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +848,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +856,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +864,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,7 +872,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,7 +880,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -912,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -920,7 +896,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -928,7 +904,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +912,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -944,7 +920,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,39 +928,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>